<commit_message>
Build out Modifiers, Business Units
</commit_message>
<xml_diff>
--- a/Documentation/Transaction Codes.xlsx
+++ b/Documentation/Transaction Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KennyHawkins\Documents\Canal\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5996D07B-9565-4234-BF7A-AC78B4990A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2945A7-F84B-4CFF-802C-019D665B1DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31140" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{B4990264-3A6B-44C5-97BD-91A98D01CBB8}"/>
   </bookViews>
@@ -39,10 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="161">
-  <si>
-    <t>Module</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="165">
   <si>
     <t>Description</t>
   </si>
@@ -50,9 +47,6 @@
     <t>/</t>
   </si>
   <si>
-    <t>Controller (All Available Actions)</t>
-  </si>
-  <si>
     <t>/CATS</t>
   </si>
   <si>
@@ -522,6 +516,24 @@
   </si>
   <si>
     <t>List of Organizations or find with Org ID</t>
+  </si>
+  <si>
+    <t>/WHS/MOD</t>
+  </si>
+  <si>
+    <t>Modify a Warehouse</t>
+  </si>
+  <si>
+    <t>/ORGS/MOD</t>
+  </si>
+  <si>
+    <t>Modify an Organization</t>
+  </si>
+  <si>
+    <t>Module/Canal/Tr. Code</t>
+  </si>
+  <si>
+    <t>Controller (All Available Actions, Always Open)</t>
   </si>
 </sst>
 </file>
@@ -909,665 +921,681 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C14EEF4-8523-4B58-8E08-5E0D41EFADDB}">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B46" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B48" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B49" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B50" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B51" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B52" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B53" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B54" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B55" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B56" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B57" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B59" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B60" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B61" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B62" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B63" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B64" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B65" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>112</v>
+        <v>161</v>
       </c>
       <c r="B66" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B67" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B68" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B69" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B70" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B71" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B72" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B73" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B74" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B75" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B76" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B77" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B78" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B79" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B80" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B81" t="s">
-        <v>142</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B82" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B83" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
...continued, and good night!
</commit_message>
<xml_diff>
--- a/Documentation/Transaction Codes.xlsx
+++ b/Documentation/Transaction Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KennyHawkins\Documents\Canal\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2945A7-F84B-4CFF-802C-019D665B1DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15254B8-8D8E-4948-ACDF-9A733D52ACA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31140" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{B4990264-3A6B-44C5-97BD-91A98D01CBB8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="173">
   <si>
     <t>Description</t>
   </si>
@@ -534,6 +534,30 @@
   </si>
   <si>
     <t>Controller (All Available Actions, Always Open)</t>
+  </si>
+  <si>
+    <t>/DPTS</t>
+  </si>
+  <si>
+    <t>/DPTS/F</t>
+  </si>
+  <si>
+    <t>/DPTS/NEW</t>
+  </si>
+  <si>
+    <t>/DPTS/MOD</t>
+  </si>
+  <si>
+    <t>Modify a Department</t>
+  </si>
+  <si>
+    <t>Create a Department</t>
+  </si>
+  <si>
+    <t>Find a Department with Name or ID</t>
+  </si>
+  <si>
+    <t>List of Departments of Org</t>
   </si>
 </sst>
 </file>
@@ -921,11 +945,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C14EEF4-8523-4B58-8E08-5E0D41EFADDB}">
-  <dimension ref="A1:B83"/>
+  <dimension ref="A1:B87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,551 +1080,583 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>165</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>166</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>168</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>167</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B42" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>141</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>150</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>142</v>
+        <v>86</v>
       </c>
       <c r="B49" t="s">
-        <v>151</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>143</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>152</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>144</v>
+        <v>90</v>
       </c>
       <c r="B51" t="s">
-        <v>153</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B52" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B53" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B54" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B55" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>92</v>
+        <v>148</v>
       </c>
       <c r="B56" t="s">
-        <v>93</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>94</v>
+        <v>145</v>
       </c>
       <c r="B57" t="s">
-        <v>95</v>
+        <v>154</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>96</v>
+        <v>146</v>
       </c>
       <c r="B58" t="s">
-        <v>97</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="B59" t="s">
-        <v>99</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B60" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B61" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B62" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B63" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>157</v>
+        <v>100</v>
       </c>
       <c r="B64" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B65" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>161</v>
+        <v>104</v>
       </c>
       <c r="B66" t="s">
-        <v>162</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B67" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>112</v>
+        <v>157</v>
       </c>
       <c r="B68" t="s">
-        <v>113</v>
+        <v>158</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="B69" t="s">
-        <v>115</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B70" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B71" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B72" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B73" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B74" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B75" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B76" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B77" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B78" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B79" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B80" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B81" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B82" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B83" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B84" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B85" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B86" t="s">
         <v>160</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B87" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{96BBBF05-C596-4D1F-AA07-A6A23ADFC26F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B72">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B87">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Minor enhancements and stubs
</commit_message>
<xml_diff>
--- a/Documentation/Transaction Codes.xlsx
+++ b/Documentation/Transaction Codes.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KennyHawkins\Documents\Canal\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15254B8-8D8E-4948-ACDF-9A733D52ACA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57081414-E3AB-46E0-B9CE-4064A9C23145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31140" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{B4990264-3A6B-44C5-97BD-91A98D01CBB8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Available Modules" sheetId="1" r:id="rId1"/>
+    <sheet name="Available Canals" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Available Modules'!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Available Canals'!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="179">
   <si>
     <t>Description</t>
   </si>
@@ -558,13 +558,31 @@
   </si>
   <si>
     <t>List of Departments of Org</t>
+  </si>
+  <si>
+    <t>/CLEAR_DSK</t>
+  </si>
+  <si>
+    <t>Minimizes all Windows</t>
+  </si>
+  <si>
+    <t>/CLOSE_DSK</t>
+  </si>
+  <si>
+    <t>Closes all windows, no confirmation</t>
+  </si>
+  <si>
+    <t>/CNL</t>
+  </si>
+  <si>
+    <t>Canal Interface Settings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -575,6 +593,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -607,10 +640,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -945,718 +980,742 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C14EEF4-8523-4B58-8E08-5E0D41EFADDB}">
-  <dimension ref="A1:B87"/>
+  <dimension ref="A1:B90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B18" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B32" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B33" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B34" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B35" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B36" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B39" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B40" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+    <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B41" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B42" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B43" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B44" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B45" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+    <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B46" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B47" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+    <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B48" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B49" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B50" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B51" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B52" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B53" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B54" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+    <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B55" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B56" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+    <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B57" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B58" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+    <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B59" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B60" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B61" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+    <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B62" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+    <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B63" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+    <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B64" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+    <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B65" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+    <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B66" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+    <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B67" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+    <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B68" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+    <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B69" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B70" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+    <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B71" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+    <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B72" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+    <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B73" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+    <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B74" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+    <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B75" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+    <row r="76" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B76" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+    <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B77" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+    <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B78" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+    <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B79" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+    <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B80" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+    <row r="81" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B81" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+    <row r="82" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B82" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
+    <row r="83" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B83" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
+    <row r="84" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B84" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+    <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B85" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
+    <row r="86" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B86" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
+    <row r="87" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B87" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+    <row r="88" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B88" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
+    <row r="89" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B89" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
+    <row r="90" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B90" s="4" t="s">
         <v>140</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{96BBBF05-C596-4D1F-AA07-A6A23ADFC26F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B87">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B90">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Building feature base still
</commit_message>
<xml_diff>
--- a/Documentation/Transaction Codes.xlsx
+++ b/Documentation/Transaction Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KennyHawkins\Documents\Canal\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F522DC-1B6A-448F-84E3-E0846B9C11A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F687AE9F-B141-4C56-B11A-CDA0C265BC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B4990264-3A6B-44C5-97BD-91A98D01CBB8}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Available Canals" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Available Canals'!$A$1:$M$116</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Available Canals'!$A$1:$M$122</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="264">
   <si>
     <t>/</t>
   </si>
@@ -428,9 +428,6 @@
     <t>Find Vendor with ID</t>
   </si>
   <si>
-    <t>Find Vendor with Vendor ID</t>
-  </si>
-  <si>
     <t>/VEND/MOD</t>
   </si>
   <si>
@@ -792,6 +789,48 @@
   </si>
   <si>
     <t>Manager SimpleForms in this window (create, mod, del)</t>
+  </si>
+  <si>
+    <t>/MVMT/TSKS</t>
+  </si>
+  <si>
+    <t>/MVMT/TSKS/F</t>
+  </si>
+  <si>
+    <t>Task list for all users</t>
+  </si>
+  <si>
+    <t>Find Task by various Task properties</t>
+  </si>
+  <si>
+    <t>/MVMT/TSKS/NEW</t>
+  </si>
+  <si>
+    <t>Create new Task for User</t>
+  </si>
+  <si>
+    <t>/MVMT/WVS</t>
+  </si>
+  <si>
+    <t>/MVMT/WVS/F</t>
+  </si>
+  <si>
+    <t>/MVMT/WVS/NEW</t>
+  </si>
+  <si>
+    <t>List of Waves for all locations</t>
+  </si>
+  <si>
+    <t>Find Wave with Wave ID</t>
+  </si>
+  <si>
+    <t>Create a Wave for Location</t>
+  </si>
+  <si>
+    <t>/VEND/ARCVH</t>
+  </si>
+  <si>
+    <t>Archive a Vendor with ID</t>
   </si>
 </sst>
 </file>
@@ -1331,11 +1370,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C14EEF4-8523-4B58-8E08-5E0D41EFADDB}">
-  <dimension ref="A1:M116"/>
+  <dimension ref="A1:M122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,43 +1396,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="M1" s="13" t="s">
         <v>185</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -1401,38 +1440,38 @@
         <v>0</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -1444,25 +1483,25 @@
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M3" s="13"/>
     </row>
@@ -1474,13 +1513,13 @@
         <v>4</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -1489,7 +1528,7 @@
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M4" s="13"/>
     </row>
@@ -1502,23 +1541,23 @@
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M5" s="13"/>
     </row>
@@ -1531,21 +1570,21 @@
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M6" s="13"/>
     </row>
@@ -1558,37 +1597,37 @@
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M7" s="13"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>214</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>215</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
@@ -1601,16 +1640,16 @@
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="B9" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>210</v>
-      </c>
       <c r="C9" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
@@ -1624,19 +1663,19 @@
     </row>
     <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>208</v>
-      </c>
       <c r="C10" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -1656,37 +1695,37 @@
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
@@ -1706,142 +1745,142 @@
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>171</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>172</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M14" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>173</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>174</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L15" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B16" s="19" t="s">
         <v>175</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>176</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M16" s="13"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>199</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>200</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
@@ -1854,19 +1893,19 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="C18" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>203</v>
-      </c>
       <c r="D18" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
@@ -1879,19 +1918,19 @@
     </row>
     <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="C19" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>194</v>
-      </c>
       <c r="D19" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
@@ -1904,13 +1943,13 @@
     </row>
     <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="C20" s="16" t="s">
         <v>249</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>250</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
@@ -1932,29 +1971,29 @@
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K21" s="12"/>
       <c r="L21" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M21" s="13"/>
     </row>
@@ -1967,29 +2006,29 @@
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K22" s="12"/>
       <c r="L22" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M22" s="13"/>
     </row>
@@ -2002,29 +2041,29 @@
       </c>
       <c r="C23" s="16"/>
       <c r="D23" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K23" s="12"/>
       <c r="L23" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M23" s="13"/>
     </row>
@@ -2037,21 +2076,21 @@
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
       <c r="H24" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M24" s="13"/>
     </row>
@@ -2064,21 +2103,21 @@
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
       <c r="H25" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M25" s="13"/>
     </row>
@@ -2091,63 +2130,63 @@
       </c>
       <c r="C26" s="16"/>
       <c r="D26" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M26" s="13"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M27" s="13"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="B28" s="19" t="s">
-        <v>217</v>
-      </c>
       <c r="C28" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
@@ -2161,19 +2200,19 @@
     </row>
     <row r="29" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>205</v>
-      </c>
       <c r="C29" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
@@ -2186,82 +2225,82 @@
     </row>
     <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C30" s="16"/>
       <c r="D30" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
       <c r="H30" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
       <c r="L30" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M30" s="13"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B31" s="19" t="s">
         <v>166</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>167</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
       <c r="H31" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
       <c r="L31" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M31" s="13"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C32" s="16"/>
       <c r="D32" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
       <c r="H32" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
       <c r="L32" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M32" s="13"/>
     </row>
@@ -2274,21 +2313,21 @@
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
       <c r="H33" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
       <c r="L33" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M33" s="13"/>
     </row>
@@ -2300,13 +2339,13 @@
         <v>30</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
@@ -2315,7 +2354,7 @@
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
       <c r="L34" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M34" s="13"/>
     </row>
@@ -2328,21 +2367,21 @@
       </c>
       <c r="C35" s="16"/>
       <c r="D35" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
       <c r="L35" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M35" s="13"/>
     </row>
@@ -2355,21 +2394,21 @@
       </c>
       <c r="C36" s="16"/>
       <c r="D36" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
       <c r="H36" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M36" s="13"/>
     </row>
@@ -2382,37 +2421,37 @@
       </c>
       <c r="C37" s="16"/>
       <c r="D37" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M37" s="13"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="B38" s="19" t="s">
         <v>218</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>219</v>
       </c>
       <c r="C38" s="16"/>
       <c r="D38" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
@@ -2420,23 +2459,23 @@
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
       <c r="K38" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L38" s="12"/>
       <c r="M38" s="13"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="B39" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="B39" s="19" t="s">
-        <v>226</v>
-      </c>
       <c r="C39" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
@@ -2445,26 +2484,26 @@
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
       <c r="K39" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L39" s="12"/>
       <c r="M39" s="13"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
@@ -2477,15 +2516,15 @@
     </row>
     <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B41" s="19"/>
       <c r="C41" s="16"/>
       <c r="D41" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
@@ -2493,24 +2532,24 @@
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
       <c r="K41" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L41" s="12"/>
       <c r="M41" s="13"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C42" s="16"/>
       <c r="D42" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
@@ -2518,24 +2557,24 @@
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
       <c r="K42" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L42" s="12"/>
       <c r="M42" s="13"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>220</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>221</v>
       </c>
       <c r="C43" s="16"/>
       <c r="D43" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
@@ -2543,24 +2582,24 @@
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
       <c r="K43" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L43" s="12"/>
       <c r="M43" s="13"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>229</v>
-      </c>
-      <c r="B44" s="19" t="s">
-        <v>230</v>
       </c>
       <c r="C44" s="16"/>
       <c r="D44" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
@@ -2568,26 +2607,26 @@
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
       <c r="K44" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L44" s="12"/>
       <c r="M44" s="13"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>190</v>
-      </c>
       <c r="C45" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
@@ -2607,21 +2646,21 @@
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
       <c r="L46" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M46" s="13"/>
     </row>
@@ -2634,21 +2673,21 @@
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
       <c r="H47" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
       <c r="K47" s="12"/>
       <c r="L47" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M47" s="13"/>
     </row>
@@ -2661,21 +2700,21 @@
       </c>
       <c r="C48" s="16"/>
       <c r="D48" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
       <c r="H48" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M48" s="13"/>
     </row>
@@ -2688,21 +2727,21 @@
       </c>
       <c r="C49" s="16"/>
       <c r="D49" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
       <c r="H49" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M49" s="13"/>
     </row>
@@ -2715,21 +2754,21 @@
       </c>
       <c r="C50" s="16"/>
       <c r="D50" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
       <c r="H50" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
       <c r="K50" s="12"/>
       <c r="L50" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M50" s="13"/>
     </row>
@@ -2742,21 +2781,21 @@
       </c>
       <c r="C51" s="16"/>
       <c r="D51" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
       <c r="H51" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
       <c r="L51" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M51" s="13"/>
     </row>
@@ -2769,36 +2808,36 @@
       </c>
       <c r="C52" s="16"/>
       <c r="D52" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
       <c r="H52" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
       <c r="L52" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M52" s="13"/>
     </row>
     <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="B53" s="19" t="s">
         <v>236</v>
-      </c>
-      <c r="B53" s="19" t="s">
-        <v>237</v>
       </c>
       <c r="C53" s="16"/>
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
       <c r="F53" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G53" s="12"/>
       <c r="H53" s="12"/>
@@ -2810,18 +2849,18 @@
     </row>
     <row r="54" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="B54" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="B54" s="19" t="s">
+      <c r="C54" s="16" t="s">
         <v>245</v>
-      </c>
-      <c r="C54" s="16" t="s">
-        <v>246</v>
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
       <c r="F54" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G54" s="12"/>
       <c r="H54" s="12"/>
@@ -2833,16 +2872,16 @@
     </row>
     <row r="55" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="B55" s="19" t="s">
         <v>242</v>
-      </c>
-      <c r="B55" s="19" t="s">
-        <v>243</v>
       </c>
       <c r="C55" s="16"/>
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
       <c r="F55" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G55" s="12"/>
       <c r="H55" s="12"/>
@@ -2854,16 +2893,16 @@
     </row>
     <row r="56" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B56" s="19" t="s">
         <v>240</v>
-      </c>
-      <c r="B56" s="19" t="s">
-        <v>241</v>
       </c>
       <c r="C56" s="16"/>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
       <c r="F56" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
@@ -2875,16 +2914,16 @@
     </row>
     <row r="57" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="B57" s="19" t="s">
         <v>238</v>
-      </c>
-      <c r="B57" s="19" t="s">
-        <v>239</v>
       </c>
       <c r="C57" s="16"/>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
@@ -2896,13 +2935,13 @@
     </row>
     <row r="58" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="B58" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="B58" s="19" t="s">
+      <c r="C58" s="16" t="s">
         <v>232</v>
-      </c>
-      <c r="C58" s="16" t="s">
-        <v>233</v>
       </c>
       <c r="D58" s="12"/>
       <c r="E58" s="12"/>
@@ -2924,21 +2963,21 @@
       </c>
       <c r="C59" s="16"/>
       <c r="D59" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
       <c r="H59" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I59" s="12"/>
       <c r="J59" s="12"/>
       <c r="K59" s="12"/>
       <c r="L59" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M59" s="13"/>
     </row>
@@ -2950,13 +2989,13 @@
         <v>54</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
@@ -2965,7 +3004,7 @@
       <c r="J60" s="12"/>
       <c r="K60" s="12"/>
       <c r="L60" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M60" s="13"/>
     </row>
@@ -2978,21 +3017,21 @@
       </c>
       <c r="C61" s="16"/>
       <c r="D61" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
       <c r="H61" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
       <c r="K61" s="12"/>
       <c r="L61" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M61" s="13"/>
     </row>
@@ -3005,21 +3044,21 @@
       </c>
       <c r="C62" s="16"/>
       <c r="D62" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
       <c r="H62" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I62" s="12"/>
       <c r="J62" s="12"/>
       <c r="K62" s="12"/>
       <c r="L62" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M62" s="13"/>
     </row>
@@ -3032,1167 +3071,1129 @@
       </c>
       <c r="C63" s="16"/>
       <c r="D63" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
       <c r="H63" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
       <c r="K63" s="12"/>
       <c r="L63" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M63" s="13"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>61</v>
+        <v>250</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>62</v>
+        <v>252</v>
       </c>
       <c r="C64" s="16"/>
-      <c r="D64" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F64" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
       <c r="G64" s="12"/>
-      <c r="H64" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="H64" s="12"/>
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
       <c r="K64" s="12"/>
-      <c r="L64" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="L64" s="12"/>
       <c r="M64" s="13"/>
     </row>
     <row r="65" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>63</v>
+        <v>251</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C65" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="E65" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F65" s="12" t="s">
-        <v>178</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="C65" s="16"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
       <c r="G65" s="12"/>
       <c r="H65" s="12"/>
       <c r="I65" s="12"/>
       <c r="J65" s="12"/>
       <c r="K65" s="12"/>
-      <c r="L65" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="L65" s="12"/>
       <c r="M65" s="13"/>
     </row>
     <row r="66" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>65</v>
+        <v>254</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>66</v>
+        <v>255</v>
       </c>
       <c r="C66" s="16"/>
-      <c r="D66" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F66" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
       <c r="G66" s="12"/>
-      <c r="H66" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="H66" s="12"/>
       <c r="I66" s="12"/>
       <c r="J66" s="12"/>
       <c r="K66" s="12"/>
-      <c r="L66" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="L66" s="12"/>
       <c r="M66" s="13"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>67</v>
+        <v>256</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>68</v>
+        <v>259</v>
       </c>
       <c r="C67" s="16"/>
-      <c r="D67" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="E67" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F67" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
       <c r="G67" s="12"/>
-      <c r="H67" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="H67" s="12"/>
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
       <c r="K67" s="12"/>
-      <c r="L67" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="L67" s="12"/>
       <c r="M67" s="13"/>
     </row>
     <row r="68" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>69</v>
+        <v>257</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="C68" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="D68" s="12" t="s">
-        <v>178</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="C68" s="16"/>
+      <c r="D68" s="12"/>
       <c r="E68" s="12"/>
-      <c r="F68" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="F68" s="12"/>
       <c r="G68" s="12"/>
-      <c r="H68" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="H68" s="12"/>
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
       <c r="K68" s="12"/>
-      <c r="L68" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="L68" s="12"/>
       <c r="M68" s="13"/>
     </row>
     <row r="69" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>71</v>
+        <v>258</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="C69" s="16"/>
-      <c r="D69" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F69" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
       <c r="G69" s="12"/>
-      <c r="H69" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="H69" s="12"/>
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
       <c r="K69" s="12"/>
-      <c r="L69" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="L69" s="12"/>
       <c r="M69" s="13"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C70" s="16"/>
       <c r="D70" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F70" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G70" s="12"/>
       <c r="H70" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I70" s="12"/>
       <c r="J70" s="12"/>
       <c r="K70" s="12"/>
       <c r="L70" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M70" s="13"/>
     </row>
     <row r="71" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C71" s="16"/>
+        <v>64</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>210</v>
+      </c>
       <c r="D71" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F71" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G71" s="12"/>
-      <c r="H71" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="H71" s="12"/>
       <c r="I71" s="12"/>
       <c r="J71" s="12"/>
       <c r="K71" s="12"/>
       <c r="L71" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M71" s="13"/>
     </row>
     <row r="72" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C72" s="16"/>
       <c r="D72" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F72" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G72" s="12"/>
       <c r="H72" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I72" s="12"/>
       <c r="J72" s="12"/>
       <c r="K72" s="12"/>
       <c r="L72" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M72" s="13"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C73" s="16" t="s">
-        <v>212</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C73" s="16"/>
       <c r="D73" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="E73" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="F73" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G73" s="12"/>
       <c r="H73" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I73" s="12"/>
       <c r="J73" s="12"/>
       <c r="K73" s="12"/>
       <c r="L73" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M73" s="13"/>
     </row>
     <row r="74" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C74" s="16"/>
+        <v>70</v>
+      </c>
+      <c r="C74" s="16" t="s">
+        <v>211</v>
+      </c>
       <c r="D74" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="E74" s="12" t="s">
-        <v>178</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="E74" s="12"/>
       <c r="F74" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G74" s="12"/>
       <c r="H74" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I74" s="12"/>
       <c r="J74" s="12"/>
       <c r="K74" s="12"/>
       <c r="L74" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M74" s="13"/>
     </row>
     <row r="75" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="C75" s="16" t="s">
-        <v>211</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="C75" s="16"/>
       <c r="D75" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F75" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G75" s="12"/>
-      <c r="H75" s="12"/>
+      <c r="H75" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="I75" s="12"/>
       <c r="J75" s="12"/>
       <c r="K75" s="12"/>
       <c r="L75" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M75" s="13"/>
     </row>
     <row r="76" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C76" s="16"/>
       <c r="D76" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F76" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G76" s="12"/>
       <c r="H76" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I76" s="12"/>
       <c r="J76" s="12"/>
       <c r="K76" s="12"/>
       <c r="L76" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M76" s="13"/>
     </row>
     <row r="77" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C77" s="16"/>
       <c r="D77" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G77" s="12"/>
       <c r="H77" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I77" s="12"/>
       <c r="J77" s="12"/>
       <c r="K77" s="12"/>
       <c r="L77" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M77" s="13"/>
     </row>
     <row r="78" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C78" s="16"/>
       <c r="D78" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E78" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F78" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G78" s="12"/>
       <c r="H78" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I78" s="12"/>
       <c r="J78" s="12"/>
       <c r="K78" s="12"/>
       <c r="L78" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M78" s="13"/>
     </row>
     <row r="79" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="C79" s="16"/>
+        <v>80</v>
+      </c>
+      <c r="C79" s="16" t="s">
+        <v>211</v>
+      </c>
       <c r="D79" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="E79" s="12" t="s">
-        <v>178</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="E79" s="12"/>
       <c r="F79" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G79" s="12"/>
       <c r="H79" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I79" s="12"/>
       <c r="J79" s="12"/>
       <c r="K79" s="12"/>
       <c r="L79" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M79" s="13"/>
     </row>
     <row r="80" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>141</v>
+        <v>81</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="C80" s="16" t="s">
-        <v>212</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="C80" s="16"/>
       <c r="D80" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="E80" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="E80" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="F80" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G80" s="12"/>
-      <c r="H80" s="12"/>
+      <c r="H80" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="I80" s="12"/>
       <c r="J80" s="12"/>
       <c r="K80" s="12"/>
       <c r="L80" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M80" s="13"/>
     </row>
     <row r="81" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
-        <v>142</v>
+        <v>83</v>
       </c>
       <c r="B81" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="C81" s="16"/>
+        <v>84</v>
+      </c>
+      <c r="C81" s="16" t="s">
+        <v>210</v>
+      </c>
       <c r="D81" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E81" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F81" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G81" s="12"/>
-      <c r="H81" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="H81" s="12"/>
       <c r="I81" s="12"/>
       <c r="J81" s="12"/>
       <c r="K81" s="12"/>
       <c r="L81" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M81" s="13"/>
     </row>
     <row r="82" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="B82" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="C82" s="16" t="s">
-        <v>211</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="C82" s="16"/>
       <c r="D82" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E82" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F82" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G82" s="12"/>
-      <c r="H82" s="12"/>
+      <c r="H82" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="I82" s="12"/>
       <c r="J82" s="12"/>
       <c r="K82" s="12"/>
       <c r="L82" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M82" s="13"/>
     </row>
     <row r="83" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
-        <v>147</v>
+        <v>87</v>
       </c>
       <c r="B83" s="19" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="C83" s="16"/>
       <c r="D83" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E83" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F83" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G83" s="12"/>
       <c r="H83" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I83" s="12"/>
       <c r="J83" s="12"/>
       <c r="K83" s="12"/>
       <c r="L83" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M83" s="13"/>
     </row>
     <row r="84" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
-        <v>144</v>
+        <v>89</v>
       </c>
       <c r="B84" s="19" t="s">
-        <v>153</v>
+        <v>90</v>
       </c>
       <c r="C84" s="16"/>
       <c r="D84" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F84" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G84" s="12"/>
       <c r="H84" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I84" s="12"/>
       <c r="J84" s="12"/>
       <c r="K84" s="12"/>
       <c r="L84" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M84" s="13"/>
     </row>
     <row r="85" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B85" s="19" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C85" s="16"/>
       <c r="D85" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F85" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G85" s="12"/>
       <c r="H85" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I85" s="12"/>
       <c r="J85" s="12"/>
       <c r="K85" s="12"/>
       <c r="L85" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M85" s="13"/>
     </row>
     <row r="86" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B86" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="C86" s="16"/>
+        <v>149</v>
+      </c>
+      <c r="C86" s="16" t="s">
+        <v>211</v>
+      </c>
       <c r="D86" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="E86" s="12" t="s">
-        <v>178</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="E86" s="12"/>
       <c r="F86" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G86" s="12"/>
-      <c r="H86" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="H86" s="12"/>
       <c r="I86" s="12"/>
       <c r="J86" s="12"/>
       <c r="K86" s="12"/>
       <c r="L86" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M86" s="13"/>
     </row>
     <row r="87" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>91</v>
+        <v>141</v>
       </c>
       <c r="B87" s="19" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
       <c r="C87" s="16"/>
       <c r="D87" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E87" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F87" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G87" s="12"/>
       <c r="H87" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I87" s="12"/>
       <c r="J87" s="12"/>
       <c r="K87" s="12"/>
       <c r="L87" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M87" s="13"/>
     </row>
     <row r="88" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
       <c r="B88" s="19" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="C88" s="16" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D88" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="E88" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="E88" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="F88" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G88" s="12"/>
-      <c r="H88" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="H88" s="12"/>
       <c r="I88" s="12"/>
       <c r="J88" s="12"/>
       <c r="K88" s="12"/>
       <c r="L88" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M88" s="13"/>
     </row>
     <row r="89" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>95</v>
+        <v>146</v>
       </c>
       <c r="B89" s="19" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
       <c r="C89" s="16"/>
       <c r="D89" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E89" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F89" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G89" s="12"/>
       <c r="H89" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I89" s="12"/>
       <c r="J89" s="12"/>
       <c r="K89" s="12"/>
       <c r="L89" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M89" s="13"/>
     </row>
     <row r="90" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>97</v>
+        <v>143</v>
       </c>
       <c r="B90" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="C90" s="16" t="s">
-        <v>211</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="C90" s="16"/>
       <c r="D90" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E90" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F90" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G90" s="12"/>
-      <c r="H90" s="12"/>
+      <c r="H90" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="I90" s="12"/>
       <c r="J90" s="12"/>
       <c r="K90" s="12"/>
       <c r="L90" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M90" s="13"/>
     </row>
     <row r="91" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
       <c r="B91" s="19" t="s">
-        <v>100</v>
+        <v>153</v>
       </c>
       <c r="C91" s="16"/>
       <c r="D91" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E91" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F91" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G91" s="12"/>
       <c r="H91" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I91" s="12"/>
       <c r="J91" s="12"/>
       <c r="K91" s="12"/>
       <c r="L91" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M91" s="13"/>
     </row>
     <row r="92" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>101</v>
+        <v>145</v>
       </c>
       <c r="B92" s="19" t="s">
-        <v>102</v>
+        <v>154</v>
       </c>
       <c r="C92" s="16"/>
       <c r="D92" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E92" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F92" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G92" s="12"/>
       <c r="H92" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I92" s="12"/>
       <c r="J92" s="12"/>
       <c r="K92" s="12"/>
       <c r="L92" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M92" s="13"/>
     </row>
     <row r="93" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B93" s="19" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C93" s="16"/>
       <c r="D93" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E93" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F93" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G93" s="12"/>
       <c r="H93" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I93" s="12"/>
       <c r="J93" s="12"/>
       <c r="K93" s="12"/>
       <c r="L93" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M93" s="13"/>
     </row>
     <row r="94" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B94" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C94" s="16"/>
+        <v>94</v>
+      </c>
+      <c r="C94" s="16" t="s">
+        <v>211</v>
+      </c>
       <c r="D94" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="E94" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F94" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="G94" s="12"/>
       <c r="H94" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I94" s="12"/>
       <c r="J94" s="12"/>
       <c r="K94" s="12"/>
       <c r="L94" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M94" s="13"/>
     </row>
     <row r="95" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
-        <v>156</v>
+        <v>95</v>
       </c>
       <c r="B95" s="19" t="s">
-        <v>157</v>
+        <v>96</v>
       </c>
       <c r="C95" s="16"/>
       <c r="D95" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F95" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="F95" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="G95" s="12"/>
       <c r="H95" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I95" s="12"/>
       <c r="J95" s="12"/>
       <c r="K95" s="12"/>
       <c r="L95" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M95" s="13"/>
     </row>
     <row r="96" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
-        <v>160</v>
+        <v>97</v>
       </c>
       <c r="B96" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="C96" s="16"/>
+        <v>98</v>
+      </c>
+      <c r="C96" s="16" t="s">
+        <v>210</v>
+      </c>
       <c r="D96" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E96" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F96" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="F96" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="G96" s="12"/>
-      <c r="H96" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="H96" s="12"/>
       <c r="I96" s="12"/>
       <c r="J96" s="12"/>
       <c r="K96" s="12"/>
       <c r="L96" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M96" s="13"/>
     </row>
     <row r="97" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C97" s="16"/>
       <c r="D97" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E97" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F97" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="F97" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="G97" s="12"/>
       <c r="H97" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I97" s="12"/>
       <c r="J97" s="12"/>
       <c r="K97" s="12"/>
       <c r="L97" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M97" s="13"/>
     </row>
     <row r="98" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
-        <v>196</v>
+        <v>101</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="C98" s="16" t="s">
-        <v>198</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="C98" s="16"/>
       <c r="D98" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E98" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F98" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="F98" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="G98" s="12"/>
-      <c r="H98" s="12"/>
+      <c r="H98" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="I98" s="12"/>
       <c r="J98" s="12"/>
       <c r="K98" s="12"/>
-      <c r="L98" s="12"/>
+      <c r="L98" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="M98" s="13"/>
     </row>
     <row r="99" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C99" s="16"/>
       <c r="D99" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E99" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F99" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="F99" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="G99" s="12"/>
       <c r="H99" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I99" s="12"/>
       <c r="J99" s="12"/>
       <c r="K99" s="12"/>
       <c r="L99" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M99" s="13"/>
     </row>
     <row r="100" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="21" t="s">
-        <v>234</v>
+      <c r="A100" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>235</v>
+        <v>106</v>
       </c>
       <c r="C100" s="16"/>
-      <c r="D100" s="12"/>
-      <c r="E100" s="12"/>
+      <c r="D100" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E100" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="F100" s="12"/>
       <c r="G100" s="12"/>
-      <c r="H100" s="12"/>
+      <c r="H100" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="I100" s="12"/>
       <c r="J100" s="12"/>
       <c r="K100" s="12"/>
-      <c r="L100" s="12"/>
+      <c r="L100" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="M100" s="13"/>
     </row>
     <row r="101" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
-        <v>111</v>
+        <v>155</v>
       </c>
       <c r="B101" s="19" t="s">
-        <v>112</v>
+        <v>156</v>
       </c>
       <c r="C101" s="16"/>
       <c r="D101" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E101" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F101" s="12"/>
       <c r="G101" s="12"/>
       <c r="H101" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I101" s="12"/>
       <c r="J101" s="12"/>
       <c r="K101" s="12"/>
       <c r="L101" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M101" s="13"/>
     </row>
     <row r="102" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="C102" s="16"/>
       <c r="D102" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E102" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F102" s="12"/>
       <c r="G102" s="12"/>
       <c r="H102" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I102" s="12"/>
       <c r="J102" s="12"/>
       <c r="K102" s="12"/>
       <c r="L102" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M102" s="13"/>
     </row>
     <row r="103" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C103" s="16"/>
       <c r="D103" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F103" s="12"/>
       <c r="G103" s="12"/>
       <c r="H103" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I103" s="12"/>
       <c r="J103" s="12"/>
       <c r="K103" s="12"/>
       <c r="L103" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M103" s="13"/>
     </row>
     <row r="104" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
-        <v>117</v>
+        <v>195</v>
       </c>
       <c r="B104" s="19" t="s">
-        <v>118</v>
+        <v>196</v>
       </c>
       <c r="C104" s="16" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F104" s="12"/>
       <c r="G104" s="12"/>
@@ -4200,342 +4201,494 @@
       <c r="I104" s="12"/>
       <c r="J104" s="12"/>
       <c r="K104" s="12"/>
-      <c r="L104" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="L104" s="12"/>
       <c r="M104" s="13"/>
     </row>
     <row r="105" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B105" s="19" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C105" s="16"/>
       <c r="D105" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E105" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F105" s="12"/>
       <c r="G105" s="12"/>
       <c r="H105" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I105" s="12"/>
       <c r="J105" s="12"/>
       <c r="K105" s="12"/>
       <c r="L105" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M105" s="13"/>
     </row>
     <row r="106" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="14" t="s">
-        <v>121</v>
+      <c r="A106" s="21" t="s">
+        <v>233</v>
       </c>
       <c r="B106" s="19" t="s">
-        <v>122</v>
+        <v>234</v>
       </c>
       <c r="C106" s="16"/>
-      <c r="D106" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="E106" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="D106" s="12"/>
+      <c r="E106" s="12"/>
       <c r="F106" s="12"/>
       <c r="G106" s="12"/>
-      <c r="H106" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="H106" s="12"/>
       <c r="I106" s="12"/>
       <c r="J106" s="12"/>
       <c r="K106" s="12"/>
-      <c r="L106" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="L106" s="12"/>
       <c r="M106" s="13"/>
     </row>
     <row r="107" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B107" s="19" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C107" s="16"/>
       <c r="D107" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F107" s="12"/>
       <c r="G107" s="12"/>
       <c r="H107" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I107" s="12"/>
       <c r="J107" s="12"/>
       <c r="K107" s="12"/>
       <c r="L107" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M107" s="13"/>
     </row>
     <row r="108" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B108" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="C108" s="16" t="s">
-        <v>211</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="C108" s="16"/>
       <c r="D108" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E108" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F108" s="12"/>
       <c r="G108" s="12"/>
-      <c r="H108" s="12"/>
+      <c r="H108" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="I108" s="12"/>
       <c r="J108" s="12"/>
       <c r="K108" s="12"/>
       <c r="L108" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M108" s="13"/>
     </row>
     <row r="109" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C109" s="16"/>
       <c r="D109" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E109" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F109" s="12"/>
       <c r="G109" s="12"/>
       <c r="H109" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I109" s="12"/>
       <c r="J109" s="12"/>
       <c r="K109" s="12"/>
       <c r="L109" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M109" s="13"/>
     </row>
     <row r="110" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C110" s="16"/>
+        <v>118</v>
+      </c>
+      <c r="C110" s="16" t="s">
+        <v>210</v>
+      </c>
       <c r="D110" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E110" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F110" s="12"/>
       <c r="G110" s="12"/>
-      <c r="H110" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="H110" s="12"/>
       <c r="I110" s="12"/>
       <c r="J110" s="12"/>
       <c r="K110" s="12"/>
       <c r="L110" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M110" s="13"/>
     </row>
     <row r="111" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B111" s="19" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="C111" s="16"/>
       <c r="D111" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E111" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F111" s="12"/>
       <c r="G111" s="12"/>
       <c r="H111" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I111" s="12"/>
       <c r="J111" s="12"/>
       <c r="K111" s="12"/>
       <c r="L111" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M111" s="13"/>
     </row>
     <row r="112" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B112" s="19" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C112" s="16"/>
       <c r="D112" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E112" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F112" s="12"/>
       <c r="G112" s="12"/>
       <c r="H112" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I112" s="12"/>
       <c r="J112" s="12"/>
       <c r="K112" s="12"/>
       <c r="L112" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M112" s="13"/>
     </row>
     <row r="113" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C113" s="16"/>
       <c r="D113" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E113" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F113" s="12"/>
       <c r="G113" s="12"/>
       <c r="H113" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I113" s="12"/>
       <c r="J113" s="12"/>
       <c r="K113" s="12"/>
       <c r="L113" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M113" s="13"/>
     </row>
     <row r="114" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
-        <v>136</v>
+        <v>262</v>
       </c>
       <c r="B114" s="19" t="s">
-        <v>137</v>
+        <v>263</v>
       </c>
       <c r="C114" s="16"/>
       <c r="D114" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E114" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F114" s="12"/>
       <c r="G114" s="12"/>
       <c r="H114" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I114" s="12"/>
       <c r="J114" s="12"/>
       <c r="K114" s="12"/>
       <c r="L114" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M114" s="13"/>
     </row>
     <row r="115" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="B115" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="C115" s="16"/>
+        <v>126</v>
+      </c>
+      <c r="C115" s="16" t="s">
+        <v>210</v>
+      </c>
       <c r="D115" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E115" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F115" s="12"/>
       <c r="G115" s="12"/>
-      <c r="H115" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="H115" s="12"/>
       <c r="I115" s="12"/>
       <c r="J115" s="12"/>
       <c r="K115" s="12"/>
       <c r="L115" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M115" s="13"/>
     </row>
     <row r="116" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="C116" s="16"/>
       <c r="D116" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E116" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F116" s="12"/>
       <c r="G116" s="12"/>
       <c r="H116" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I116" s="12"/>
       <c r="J116" s="12"/>
       <c r="K116" s="12"/>
       <c r="L116" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M116" s="13"/>
     </row>
+    <row r="117" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A117" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B117" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C117" s="16"/>
+      <c r="D117" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E117" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F117" s="12"/>
+      <c r="G117" s="12"/>
+      <c r="H117" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="I117" s="12"/>
+      <c r="J117" s="12"/>
+      <c r="K117" s="12"/>
+      <c r="L117" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="M117" s="13"/>
+    </row>
+    <row r="118" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A118" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B118" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C118" s="16"/>
+      <c r="D118" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E118" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F118" s="12"/>
+      <c r="G118" s="12"/>
+      <c r="H118" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="I118" s="12"/>
+      <c r="J118" s="12"/>
+      <c r="K118" s="12"/>
+      <c r="L118" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="M118" s="13"/>
+    </row>
+    <row r="119" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A119" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B119" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="C119" s="16"/>
+      <c r="D119" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E119" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F119" s="12"/>
+      <c r="G119" s="12"/>
+      <c r="H119" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="I119" s="12"/>
+      <c r="J119" s="12"/>
+      <c r="K119" s="12"/>
+      <c r="L119" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="M119" s="13"/>
+    </row>
+    <row r="120" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A120" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B120" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C120" s="16"/>
+      <c r="D120" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E120" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F120" s="12"/>
+      <c r="G120" s="12"/>
+      <c r="H120" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="I120" s="12"/>
+      <c r="J120" s="12"/>
+      <c r="K120" s="12"/>
+      <c r="L120" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="M120" s="13"/>
+    </row>
+    <row r="121" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A121" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B121" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="C121" s="16"/>
+      <c r="D121" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E121" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F121" s="12"/>
+      <c r="G121" s="12"/>
+      <c r="H121" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="I121" s="12"/>
+      <c r="J121" s="12"/>
+      <c r="K121" s="12"/>
+      <c r="L121" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="M121" s="13"/>
+    </row>
+    <row r="122" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A122" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B122" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C122" s="16"/>
+      <c r="D122" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E122" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F122" s="12"/>
+      <c r="G122" s="12"/>
+      <c r="H122" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="I122" s="12"/>
+      <c r="J122" s="12"/>
+      <c r="K122" s="12"/>
+      <c r="L122" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="M122" s="13"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M116" xr:uid="{5C14EEF4-8523-4B58-8E08-5E0D41EFADDB}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M116">
-      <sortCondition ref="A1:A116"/>
+  <autoFilter ref="A1:M122" xr:uid="{5C14EEF4-8523-4B58-8E08-5E0D41EFADDB}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M122">
+      <sortCondition ref="A1:A122"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A2:M116">
+  <conditionalFormatting sqref="A2:M122">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>

</xml_diff>